<commit_message>
Updated the pins xls.
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Platform\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78259251-4256-4EC1-9CC7-331939970FFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF36996-E1DE-47C4-810C-FD01DCE523DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="272">
   <si>
     <r>
       <rPr>
@@ -2737,6 +2737,21 @@
   </si>
   <si>
     <t>D7</t>
+  </si>
+  <si>
+    <t>SWCLK</t>
+  </si>
+  <si>
+    <t>SWDIO</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
+  </si>
+  <si>
+    <t>SPI</t>
   </si>
 </sst>
 </file>
@@ -2834,12 +2849,24 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -2902,7 +2929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2958,9 +2985,6 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2972,6 +2996,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3290,7 +3329,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="S63" sqref="S63"/>
+      <selection activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3382,30 +3421,30 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="23" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="7" t="s">
         <v>19</v>
       </c>
@@ -3424,7 +3463,7 @@
       <c r="R18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="S18" s="20" t="s">
+      <c r="S18" s="19" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3438,9 +3477,9 @@
       <c r="C19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="7" t="s">
         <v>28</v>
       </c>
@@ -3465,10 +3504,10 @@
       <c r="N19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O19" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="P19" s="19"/>
+      <c r="P19" s="23"/>
       <c r="Q19" s="7" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3550,7 @@
       </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="22" t="s">
         <v>259</v>
       </c>
     </row>
@@ -3550,7 +3589,7 @@
       </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
-      <c r="S21" s="23" t="s">
+      <c r="S21" s="22" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3591,7 +3630,7 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
-      <c r="S22" s="23" t="s">
+      <c r="S22" s="22" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3632,12 +3671,12 @@
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
-      <c r="S23" s="23" t="s">
+      <c r="S23" s="22" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="10"/>
       <c r="C24" s="13">
         <v>5</v>
@@ -3667,10 +3706,10 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
-      <c r="S24" s="23"/>
+      <c r="S24" s="22"/>
     </row>
     <row r="25" spans="1:19" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="10"/>
       <c r="C25" s="13">
         <v>6</v>
@@ -3700,10 +3739,10 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
-      <c r="S25" s="23"/>
+      <c r="S25" s="22"/>
     </row>
     <row r="26" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="10"/>
       <c r="C26" s="13">
         <v>9</v>
@@ -3733,10 +3772,10 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
-      <c r="S26" s="23"/>
+      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="1:19" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="10"/>
       <c r="C27" s="13">
         <v>10</v>
@@ -3766,10 +3805,10 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
-      <c r="S27" s="23"/>
+      <c r="S27" s="22"/>
     </row>
     <row r="28" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="8">
         <v>7</v>
       </c>
@@ -3807,7 +3846,7 @@
       <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:19" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="8">
         <v>8</v>
       </c>
@@ -4057,7 +4096,7 @@
         <v>133</v>
       </c>
       <c r="L34" s="10"/>
-      <c r="M34" s="12" t="s">
+      <c r="M34" s="26" t="s">
         <v>134</v>
       </c>
       <c r="N34" s="12" t="s">
@@ -4069,6 +4108,9 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
+      <c r="S34" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="35" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
@@ -4101,7 +4143,7 @@
         <v>142</v>
       </c>
       <c r="L35" s="10"/>
-      <c r="M35" s="12" t="s">
+      <c r="M35" s="26" t="s">
         <v>143</v>
       </c>
       <c r="N35" s="12" t="s">
@@ -4113,6 +4155,9 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
+      <c r="S35" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="36" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
@@ -4143,7 +4188,7 @@
         <v>150</v>
       </c>
       <c r="L36" s="10"/>
-      <c r="M36" s="12" t="s">
+      <c r="M36" s="26" t="s">
         <v>151</v>
       </c>
       <c r="N36" s="12" t="s">
@@ -4157,6 +4202,9 @@
       <c r="R36" s="9" t="s">
         <v>154</v>
       </c>
+      <c r="S36" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="37" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
@@ -4187,7 +4235,7 @@
         <v>159</v>
       </c>
       <c r="L37" s="10"/>
-      <c r="M37" s="12" t="s">
+      <c r="M37" s="26" t="s">
         <v>160</v>
       </c>
       <c r="N37" s="12" t="s">
@@ -4201,9 +4249,12 @@
       <c r="R37" s="9" t="s">
         <v>163</v>
       </c>
+      <c r="S37" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="38" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="8">
         <v>19</v>
       </c>
@@ -4239,7 +4290,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="19.649999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="8">
         <v>20</v>
       </c>
@@ -4275,7 +4326,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8">
         <v>25</v>
@@ -4313,7 +4364,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
+      <c r="A41" s="20"/>
       <c r="B41" s="10"/>
       <c r="C41" s="8">
         <v>26</v>
@@ -4351,7 +4402,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8">
         <v>27</v>
@@ -4387,7 +4438,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="10"/>
       <c r="C43" s="8">
         <v>28</v>
@@ -4423,7 +4474,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="8">
         <v>21</v>
       </c>
@@ -4463,7 +4514,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="8">
         <v>22</v>
       </c>
@@ -4527,7 +4578,7 @@
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
-      <c r="M46" s="12" t="s">
+      <c r="M46" s="27" t="s">
         <v>152</v>
       </c>
       <c r="N46" s="12" t="s">
@@ -4540,6 +4591,9 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="11" t="s">
         <v>187</v>
+      </c>
+      <c r="S46" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
@@ -4567,7 +4621,7 @@
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
-      <c r="M47" s="12" t="s">
+      <c r="M47" s="27" t="s">
         <v>161</v>
       </c>
       <c r="N47" s="12" t="s">
@@ -4580,6 +4634,9 @@
       <c r="Q47" s="10"/>
       <c r="R47" s="11" t="s">
         <v>191</v>
+      </c>
+      <c r="S47" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
@@ -4611,7 +4668,7 @@
         <v>201</v>
       </c>
       <c r="L48" s="10"/>
-      <c r="M48" s="12" t="s">
+      <c r="M48" s="26" t="s">
         <v>42</v>
       </c>
       <c r="N48" s="12" t="s">
@@ -4625,8 +4682,11 @@
       <c r="R48" s="11" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>18</v>
       </c>
@@ -4655,7 +4715,7 @@
         <v>205</v>
       </c>
       <c r="L49" s="10"/>
-      <c r="M49" s="12" t="s">
+      <c r="M49" s="26" t="s">
         <v>47</v>
       </c>
       <c r="N49" s="12" t="s">
@@ -4669,8 +4729,11 @@
       <c r="R49" s="11" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>19</v>
       </c>
@@ -4697,7 +4760,7 @@
         <v>209</v>
       </c>
       <c r="L50" s="10"/>
-      <c r="M50" s="12" t="s">
+      <c r="M50" s="26" t="s">
         <v>210</v>
       </c>
       <c r="N50" s="12" t="s">
@@ -4711,8 +4774,11 @@
       <c r="R50" s="11" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>20</v>
       </c>
@@ -4739,7 +4805,7 @@
         <v>213</v>
       </c>
       <c r="L51" s="10"/>
-      <c r="M51" s="12" t="s">
+      <c r="M51" s="26" t="s">
         <v>214</v>
       </c>
       <c r="N51" s="12" t="s">
@@ -4753,9 +4819,12 @@
       <c r="R51" s="11" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="S51" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="21"/>
       <c r="B52" s="10"/>
       <c r="C52" s="8">
         <v>39</v>
@@ -4790,8 +4859,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8">
         <v>40</v>
@@ -4826,8 +4895,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
       <c r="B54" s="8">
         <v>29</v>
       </c>
@@ -4866,8 +4935,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
+    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
       <c r="B55" s="8">
         <v>30</v>
       </c>
@@ -4906,7 +4975,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>21</v>
       </c>
@@ -4950,7 +5019,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>22</v>
       </c>
@@ -4994,7 +5063,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>23</v>
       </c>
@@ -5032,7 +5101,7 @@
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>24</v>
       </c>
@@ -5070,8 +5139,8 @@
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
     </row>
-    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="22"/>
+    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="21"/>
       <c r="B60" s="8">
         <v>37</v>
       </c>
@@ -5106,8 +5175,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
+    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="21"/>
       <c r="B61" s="8">
         <v>38</v>
       </c>
@@ -5142,7 +5211,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>25</v>
       </c>
@@ -5176,7 +5245,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>27</v>
       </c>
@@ -5210,7 +5279,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>31</v>
       </c>
@@ -5249,8 +5318,11 @@
       <c r="R64" s="11" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S64" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="13">
         <v>32</v>
       </c>
@@ -5287,8 +5359,11 @@
         <v>243</v>
       </c>
       <c r="R65" s="10"/>
-    </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="S65" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="8">
@@ -5322,7 +5397,7 @@
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
     </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="8">
@@ -5356,7 +5431,7 @@
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
     </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8">
@@ -5392,7 +5467,7 @@
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
     </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="8">
@@ -5428,7 +5503,7 @@
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="18">
         <v>47</v>
@@ -5466,7 +5541,7 @@
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
     </row>
-    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="18">
         <v>48</v>

</xml_diff>

<commit_message>
added feedback for pin config excel sheet
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Platform\Platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELCOT\Platform\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF36996-E1DE-47C4-810C-FD01DCE523DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCB68D-46AB-43F4-8D02-B7EC3F78E5AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMD20" sheetId="1" r:id="rId1"/>
+    <sheet name="Feedback 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="295">
   <si>
     <r>
       <rPr>
@@ -120,15 +121,6 @@
         <sz val="9"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">Enable bit in the Pin Configuration register corresponding to that pin (PINCFGn.PMUXEN, n = 0-31) in the PORT </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t xml:space="preserve">must be written to one. The selection of peripheral function A to H is done by writing to the Peripheral Multiplexing </t>
     </r>
   </si>
@@ -1362,15 +1354,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA08</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>VDDIO</t>
     </r>
   </si>
@@ -1472,15 +1455,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA09</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>VDDIO</t>
     </r>
   </si>
@@ -2110,15 +2084,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>X[4]</t>
     </r>
   </si>
@@ -2153,15 +2118,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>X[5]</t>
     </r>
   </si>
@@ -2196,15 +2152,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>X[6]</t>
     </r>
   </si>
@@ -2450,15 +2397,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>X[10]</t>
     </r>
   </si>
@@ -2468,15 +2406,6 @@
         <sz val="5.5"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>PA23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="5.5"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t>X[11]</t>
     </r>
   </si>
@@ -2745,20 +2674,113 @@
     <t>SWDIO</t>
   </si>
   <si>
-    <t>I2C SDA</t>
-  </si>
-  <si>
-    <t>I2C SCL</t>
-  </si>
-  <si>
     <t>SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable bit in the Pin Configuration register corresponding to that pin (PINCFGn.PMUXEN, n = 0-31) in the PORT </t>
+  </si>
+  <si>
+    <t>PA22</t>
+  </si>
+  <si>
+    <t>PA23</t>
+  </si>
+  <si>
+    <t>PA16</t>
+  </si>
+  <si>
+    <t>PA17</t>
+  </si>
+  <si>
+    <t>PA08</t>
+  </si>
+  <si>
+    <t>PA09</t>
+  </si>
+  <si>
+    <t>PA18</t>
+  </si>
+  <si>
+    <t>I2C/SPI</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>Already Used for some other puposes</t>
+  </si>
+  <si>
+    <t>**PA15 is never used anywhere. Even in pin headers it is missing</t>
+  </si>
+  <si>
+    <t>PA14</t>
+  </si>
+  <si>
+    <t>PA30</t>
+  </si>
+  <si>
+    <t>Available for use?</t>
+  </si>
+  <si>
+    <t>PA03</t>
+  </si>
+  <si>
+    <t>PA04</t>
+  </si>
+  <si>
+    <t>PA05</t>
+  </si>
+  <si>
+    <t>PA06</t>
+  </si>
+  <si>
+    <t>PA07</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>PA24</t>
+  </si>
+  <si>
+    <t>PA25</t>
+  </si>
+  <si>
+    <t>PA27</t>
+  </si>
+  <si>
+    <t>PA28</t>
+  </si>
+  <si>
+    <t>PA00</t>
+  </si>
+  <si>
+    <t>PA01</t>
+  </si>
+  <si>
+    <t>PA02</t>
+  </si>
+  <si>
+    <t>If we want a DAC we must go to PA02</t>
+  </si>
+  <si>
+    <t>VREF can be choosen to use internal voltages</t>
+  </si>
+  <si>
+    <t>For ADC pins we have multiple options even PA08,09 can be used</t>
+  </si>
+  <si>
+    <t>PA15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2848,6 +2870,49 @@
       <sz val="5.5"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="5.5"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="5.5"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2929,7 +2994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2997,9 +3062,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -3012,6 +3074,27 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3027,6 +3110,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247034</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9176</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{178A9ACE-3D48-4812-B150-F25F89A46621}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2028825" y="457200"/>
+          <a:ext cx="4923809" cy="2790476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3328,194 +3460,194 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" customWidth="1"/>
-    <col min="6" max="6" width="4.21875" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.77734375" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
     <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.5546875" customWidth="1"/>
-    <col min="19" max="19" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
+      <c r="E18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="F18" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="O18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="P18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="Q18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="R18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="7" t="s">
+      <c r="S18" s="19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="S18" s="19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="N19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="7" t="s">
+      <c r="O19" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="O19" s="23" t="s">
+      <c r="P19" s="27"/>
+      <c r="Q19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="7" t="s">
+      <c r="R19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>1</v>
       </c>
@@ -3526,14 +3658,14 @@
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -3542,19 +3674,19 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O20" s="10"/>
       <c r="P20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>2</v>
       </c>
@@ -3565,14 +3697,14 @@
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -3581,19 +3713,19 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O21" s="10"/>
       <c r="P21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>3</v>
       </c>
@@ -3604,25 +3736,25 @@
         <v>3</v>
       </c>
       <c r="D22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
@@ -3631,10 +3763,10 @@
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="22" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="33.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>4</v>
       </c>
@@ -3645,24 +3777,24 @@
         <v>4</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="I23" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -3672,32 +3804,32 @@
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="10"/>
       <c r="C24" s="13">
         <v>5</v>
       </c>
       <c r="D24" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -3708,29 +3840,29 @@
       <c r="R24" s="10"/>
       <c r="S24" s="22"/>
     </row>
-    <row r="25" spans="1:19" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="12.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="10"/>
       <c r="C25" s="13">
         <v>6</v>
       </c>
       <c r="D25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
@@ -3741,29 +3873,29 @@
       <c r="R25" s="10"/>
       <c r="S25" s="22"/>
     </row>
-    <row r="26" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="10"/>
       <c r="C26" s="13">
         <v>9</v>
       </c>
       <c r="D26" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
@@ -3774,29 +3906,29 @@
       <c r="R26" s="10"/>
       <c r="S26" s="22"/>
     </row>
-    <row r="27" spans="1:19" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="12.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="10"/>
       <c r="C27" s="13">
         <v>10</v>
       </c>
       <c r="D27" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>77</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
@@ -3807,7 +3939,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="22"/>
     </row>
-    <row r="28" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="8">
         <v>7</v>
@@ -3816,36 +3948,36 @@
         <v>11</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O28" s="10"/>
       <c r="P28" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
     </row>
-    <row r="29" spans="1:19" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="8">
         <v>8</v>
@@ -3854,36 +3986,36 @@
         <v>12</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O29" s="10"/>
       <c r="P29" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
     </row>
-    <row r="30" spans="1:19" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>5</v>
       </c>
@@ -3894,43 +4026,43 @@
         <v>13</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="I30" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="J30" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="K30" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O30" s="10"/>
       <c r="P30" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>6</v>
       </c>
@@ -3941,41 +4073,41 @@
         <v>14</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="K31" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O31" s="10"/>
       <c r="P31" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
       <c r="S31" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>7</v>
       </c>
@@ -3986,41 +4118,41 @@
         <v>15</v>
       </c>
       <c r="D32" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="K32" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O32" s="10"/>
       <c r="P32" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
       <c r="S32" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>8</v>
       </c>
@@ -4031,41 +4163,41 @@
         <v>16</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="K33" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O33" s="10"/>
       <c r="P33" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
       <c r="S33" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>11</v>
       </c>
@@ -4075,44 +4207,44 @@
       <c r="C34" s="8">
         <v>17</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="G34" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L34" s="10"/>
+      <c r="M34" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N34" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="L34" s="10"/>
-      <c r="M34" s="26" t="s">
+      <c r="O34" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
-      <c r="S34" t="s">
+      <c r="S34" s="31" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>12</v>
       </c>
@@ -4122,44 +4254,44 @@
       <c r="C35" s="8">
         <v>18</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="L35" s="10"/>
+      <c r="M35" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="O35" s="9" t="s">
         <v>142</v>
-      </c>
-      <c r="L35" s="10"/>
-      <c r="M35" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
-      <c r="S35" t="s">
+      <c r="S35" s="31" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>13</v>
       </c>
@@ -4170,43 +4302,40 @@
         <v>19</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H36" s="10"/>
       <c r="I36" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="L36" s="10"/>
+      <c r="M36" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="O36" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="L36" s="10"/>
-      <c r="M36" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
       <c r="R36" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="S36" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>14</v>
       </c>
@@ -4217,43 +4346,40 @@
         <v>20</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="L37" s="10"/>
+      <c r="M37" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="O37" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="L37" s="10"/>
-      <c r="M37" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="N37" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
       <c r="R37" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="S37" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="8">
         <v>19</v>
@@ -4262,14 +4388,14 @@
         <v>23</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -4278,18 +4404,18 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O38" s="10"/>
       <c r="P38" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Q38" s="10"/>
       <c r="R38" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="19.649999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="19.7" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="8">
         <v>20</v>
@@ -4298,14 +4424,14 @@
         <v>24</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -4314,166 +4440,166 @@
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
       <c r="N39" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O39" s="10"/>
       <c r="P39" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="Q39" s="10"/>
       <c r="R39" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8">
         <v>25</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L40" s="10"/>
       <c r="M40" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N40" s="10"/>
       <c r="O40" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P40" s="10"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="10"/>
       <c r="C41" s="8">
         <v>26</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L41" s="10"/>
       <c r="M41" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N41" s="10"/>
       <c r="O41" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
       <c r="R41" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8">
         <v>27</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L42" s="10"/>
       <c r="M42" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="N42" s="10"/>
       <c r="O42" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
       <c r="R42" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
       <c r="B43" s="10"/>
       <c r="C43" s="8">
         <v>28</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L43" s="10"/>
       <c r="M43" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N43" s="10"/>
       <c r="O43" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
       <c r="R43" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="8">
         <v>21</v>
@@ -4482,16 +4608,16 @@
         <v>29</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
@@ -4499,21 +4625,21 @@
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
       <c r="M44" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O44" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P44" s="10"/>
       <c r="Q44" s="10"/>
       <c r="R44" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
       <c r="B45" s="8">
         <v>22</v>
@@ -4522,16 +4648,16 @@
         <v>30</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
@@ -4539,21 +4665,21 @@
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
       <c r="M45" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O45" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="10"/>
       <c r="R45" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>15</v>
       </c>
@@ -4564,39 +4690,36 @@
         <v>31</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
-      <c r="M46" s="27" t="s">
-        <v>152</v>
+      <c r="M46" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O46" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P46" s="10"/>
       <c r="Q46" s="10"/>
       <c r="R46" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="S46" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>16</v>
       </c>
@@ -4607,39 +4730,36 @@
         <v>32</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
-      <c r="M47" s="27" t="s">
-        <v>161</v>
+      <c r="M47" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="O47" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="P47" s="10"/>
       <c r="Q47" s="10"/>
       <c r="R47" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="S47" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>17</v>
       </c>
@@ -4649,44 +4769,44 @@
       <c r="C48" s="8">
         <v>35</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>200</v>
+      <c r="D48" s="29" t="s">
+        <v>265</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
       <c r="K48" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="L48" s="10"/>
-      <c r="M48" s="26" t="s">
-        <v>42</v>
+      <c r="M48" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="O48" s="10"/>
       <c r="P48" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q48" s="10"/>
       <c r="R48" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="S48" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="S48" s="31" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>18</v>
       </c>
@@ -4696,44 +4816,44 @@
       <c r="C49" s="8">
         <v>36</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>204</v>
+      <c r="D49" s="29" t="s">
+        <v>266</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
       <c r="K49" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L49" s="10"/>
-      <c r="M49" s="26" t="s">
-        <v>47</v>
+      <c r="M49" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="O49" s="10"/>
       <c r="P49" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q49" s="10"/>
       <c r="R49" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="S49" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+      <c r="S49" s="31" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>19</v>
       </c>
@@ -4743,42 +4863,42 @@
       <c r="C50" s="8">
         <v>37</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>208</v>
+      <c r="D50" s="30" t="s">
+        <v>269</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="L50" s="10"/>
-      <c r="M50" s="26" t="s">
-        <v>210</v>
+      <c r="M50" s="25" t="s">
+        <v>204</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="O50" s="10"/>
       <c r="P50" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S50" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>20</v>
       </c>
@@ -4789,57 +4909,57 @@
         <v>38</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="L51" s="10"/>
-      <c r="M51" s="26" t="s">
-        <v>214</v>
+      <c r="M51" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="O51" s="10"/>
       <c r="P51" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Q51" s="10"/>
       <c r="R51" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="S51" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="10"/>
       <c r="C52" s="8">
         <v>39</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
@@ -4847,35 +4967,35 @@
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="N52" s="10"/>
       <c r="O52" s="11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="P52" s="10"/>
       <c r="Q52" s="10"/>
       <c r="R52" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8">
         <v>40</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
@@ -4883,19 +5003,19 @@
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
       <c r="M53" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="N53" s="10"/>
       <c r="O53" s="11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="P53" s="10"/>
       <c r="Q53" s="10"/>
       <c r="R53" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="8">
         <v>29</v>
@@ -4904,38 +5024,38 @@
         <v>41</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="10"/>
       <c r="K54" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="L54" s="10"/>
       <c r="M54" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="N54" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="O54" s="11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="P54" s="10"/>
       <c r="Q54" s="10"/>
       <c r="R54" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="8">
         <v>30</v>
@@ -4944,38 +5064,38 @@
         <v>42</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
       <c r="K55" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="L55" s="10"/>
       <c r="M55" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="O55" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
       <c r="R55" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>21</v>
       </c>
@@ -4985,41 +5105,44 @@
       <c r="C56" s="8">
         <v>43</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>230</v>
+      <c r="D56" s="29" t="s">
+        <v>263</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="10"/>
       <c r="K56" s="9" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="L56" s="10"/>
       <c r="M56" s="12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="O56" s="10"/>
       <c r="P56" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q56" s="10"/>
       <c r="R56" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="S56" s="31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>22</v>
       </c>
@@ -5029,41 +5152,44 @@
       <c r="C57" s="8">
         <v>44</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>232</v>
+      <c r="D57" s="29" t="s">
+        <v>264</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="9" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="L57" s="10"/>
       <c r="M57" s="12" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="O57" s="10"/>
       <c r="P57" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q57" s="10"/>
       <c r="R57" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="S57" s="31" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>23</v>
       </c>
@@ -5074,14 +5200,14 @@
         <v>45</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
@@ -5089,19 +5215,19 @@
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
       <c r="M58" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="N58" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="O58" s="10"/>
       <c r="P58" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>24</v>
       </c>
@@ -5112,14 +5238,14 @@
         <v>46</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
@@ -5127,19 +5253,19 @@
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
       <c r="M59" s="12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N59" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="O59" s="10"/>
       <c r="P59" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="8">
         <v>37</v>
@@ -5148,14 +5274,14 @@
         <v>49</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
@@ -5164,18 +5290,18 @@
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
       <c r="N60" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="O60" s="10"/>
       <c r="P60" s="11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="Q60" s="10"/>
       <c r="R60" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="8">
         <v>38</v>
@@ -5184,14 +5310,14 @@
         <v>50</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
@@ -5200,18 +5326,18 @@
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
       <c r="N61" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="O61" s="10"/>
       <c r="P61" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Q61" s="10"/>
       <c r="R61" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>25</v>
       </c>
@@ -5222,14 +5348,14 @@
         <v>51</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F62" s="10"/>
       <c r="G62" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
@@ -5242,10 +5368,10 @@
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
       <c r="R62" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>27</v>
       </c>
@@ -5256,14 +5382,14 @@
         <v>53</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -5276,10 +5402,10 @@
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
       <c r="R63" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>31</v>
       </c>
@@ -5290,14 +5416,14 @@
         <v>57</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
@@ -5306,23 +5432,23 @@
       <c r="L64" s="10"/>
       <c r="M64" s="10"/>
       <c r="N64" s="12" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="O64" s="10"/>
       <c r="P64" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q64" s="11" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="R64" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="S64" s="24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="S64" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>32</v>
       </c>
@@ -5333,14 +5459,14 @@
         <v>58</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -5349,37 +5475,37 @@
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
       <c r="N65" s="12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="O65" s="10"/>
       <c r="P65" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q65" s="11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="R65" s="10"/>
-      <c r="S65" s="25" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+      <c r="S65" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="8">
         <v>59</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
@@ -5388,32 +5514,32 @@
       <c r="L66" s="10"/>
       <c r="M66" s="10"/>
       <c r="N66" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="O66" s="10"/>
       <c r="P66" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
     </row>
-    <row r="67" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="8">
         <v>60</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
@@ -5422,88 +5548,88 @@
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
       <c r="N67" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="O67" s="10"/>
       <c r="P67" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8">
         <v>61</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="11" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="9" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="L68" s="10"/>
       <c r="M68" s="10"/>
       <c r="N68" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="O68" s="16"/>
       <c r="P68" s="11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
     </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="8">
         <v>62</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F69" s="10"/>
       <c r="G69" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H69" s="10"/>
       <c r="I69" s="11" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J69" s="10"/>
       <c r="K69" s="9" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="L69" s="10"/>
       <c r="M69" s="10"/>
       <c r="N69" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="O69" s="16"/>
       <c r="P69" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
     </row>
-    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="18">
         <v>47</v>
@@ -5512,36 +5638,36 @@
         <v>63</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F70" s="10"/>
       <c r="G70" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="11" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="9" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="L70" s="10"/>
       <c r="M70" s="10"/>
       <c r="N70" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="O70" s="16"/>
       <c r="P70" s="11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
     </row>
-    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="18">
         <v>48</v>
@@ -5550,31 +5676,31 @@
         <v>64</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F71" s="10"/>
       <c r="G71" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="11" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="J71" s="10"/>
       <c r="K71" s="9" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L71" s="10"/>
       <c r="M71" s="10"/>
       <c r="N71" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="O71" s="16"/>
       <c r="P71" s="11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="Q71" s="10"/>
       <c r="R71" s="10"/>
@@ -5589,6 +5715,154 @@
     <mergeCell ref="H18:L18"/>
   </mergeCells>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.74583299999999997" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8F5D6-A69C-4604-B31F-611ECF924634}">
+  <dimension ref="B4:P19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="15:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="O4" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="P4" s="34" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O6" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="P7" s="35" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="P8" s="35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O9" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="P9" s="35" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="P10" s="35" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="P13" s="35" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="P14" s="35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O16" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="P16" s="36"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="O17" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="P17" s="36"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="37" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P5:P15">
+    <sortCondition ref="P5:P15"/>
+  </sortState>
+  <phoneticPr fontId="23" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Pin details# Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELCOT\Platform\Platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELCOT\Platform_2\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCB68D-46AB-43F4-8D02-B7EC3F78E5AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B31D3FC-EE30-4532-93CE-027C1659CBDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMD20" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="308">
   <si>
     <r>
       <rPr>
@@ -2774,6 +2774,45 @@
   </si>
   <si>
     <t>PA15</t>
+  </si>
+  <si>
+    <t>Pins</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C1-Digit Selection</t>
+  </si>
+  <si>
+    <t>I2C/ADC</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>SPI-CE</t>
+  </si>
+  <si>
+    <t>D2/DAC</t>
+  </si>
+  <si>
+    <t>Use it for Power Input Presence Detection</t>
   </si>
 </sst>
 </file>
@@ -2994,7 +3033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3074,9 +3113,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3091,10 +3127,22 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3458,10 +3506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q58" sqref="Q58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,6 +3533,7 @@
     <col min="17" max="17" width="6.7109375" customWidth="1"/>
     <col min="18" max="18" width="7.5703125" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -3528,7 +3577,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3553,30 +3602,30 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
       <c r="M18" s="7" t="s">
         <v>18</v>
       </c>
@@ -3609,9 +3658,9 @@
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
       <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
@@ -3636,10 +3685,10 @@
       <c r="N19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="27" t="s">
+      <c r="O19" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="27"/>
+      <c r="P19" s="36"/>
       <c r="Q19" s="7" t="s">
         <v>36</v>
       </c>
@@ -3762,8 +3811,8 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
-      <c r="S22" s="22" t="s">
-        <v>253</v>
+      <c r="S22" s="41" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4058,7 +4107,7 @@
       </c>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
-      <c r="S30" t="s">
+      <c r="S30" s="39" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4103,7 +4152,7 @@
       </c>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
-      <c r="S31" t="s">
+      <c r="S31" s="39" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4148,11 +4197,11 @@
       </c>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
-      <c r="S32" t="s">
+      <c r="S32" s="39" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>8</v>
       </c>
@@ -4193,11 +4242,11 @@
       </c>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
-      <c r="S33" t="s">
+      <c r="S33" s="39" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>11</v>
       </c>
@@ -4207,7 +4256,7 @@
       <c r="C34" s="8">
         <v>17</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="28" t="s">
         <v>267</v>
       </c>
       <c r="E34" s="9" t="s">
@@ -4240,11 +4289,11 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
-      <c r="S34" s="31" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S34" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>12</v>
       </c>
@@ -4254,7 +4303,7 @@
       <c r="C35" s="8">
         <v>18</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="28" t="s">
         <v>268</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -4287,11 +4336,11 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
-      <c r="S35" s="31" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S35" s="30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>13</v>
       </c>
@@ -4334,8 +4383,11 @@
       <c r="R36" s="9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S36" s="39" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>14</v>
       </c>
@@ -4378,8 +4430,11 @@
       <c r="R37" s="9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S37" s="39" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
       <c r="B38" s="8">
         <v>19</v>
@@ -4415,7 +4470,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="19.7" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="19.7" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="8">
         <v>20</v>
@@ -4451,7 +4506,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8">
@@ -4489,7 +4544,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="10"/>
       <c r="C41" s="8">
@@ -4527,7 +4582,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8">
@@ -4563,7 +4618,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
       <c r="B43" s="10"/>
       <c r="C43" s="8">
@@ -4599,7 +4654,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="8">
         <v>21</v>
@@ -4639,7 +4694,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20"/>
       <c r="B45" s="8">
         <v>22</v>
@@ -4679,7 +4734,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>15</v>
       </c>
@@ -4718,8 +4773,14 @@
       <c r="R46" s="11" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S46" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="T46" s="42" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>16</v>
       </c>
@@ -4758,8 +4819,11 @@
       <c r="R47" s="11" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S47" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>17</v>
       </c>
@@ -4769,7 +4833,7 @@
       <c r="C48" s="8">
         <v>35</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="28" t="s">
         <v>265</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -4802,7 +4866,7 @@
       <c r="R48" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="S48" s="31" t="s">
+      <c r="S48" s="30" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4816,7 +4880,7 @@
       <c r="C49" s="8">
         <v>36</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="28" t="s">
         <v>266</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -4849,7 +4913,7 @@
       <c r="R49" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="S49" s="31" t="s">
+      <c r="S49" s="30" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4863,7 +4927,7 @@
       <c r="C50" s="8">
         <v>37</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="29" t="s">
         <v>269</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -5105,7 +5169,7 @@
       <c r="C56" s="8">
         <v>43</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="28" t="s">
         <v>263</v>
       </c>
       <c r="E56" s="11" t="s">
@@ -5138,7 +5202,7 @@
       <c r="R56" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="S56" s="31" t="s">
+      <c r="S56" s="30" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5152,7 +5216,7 @@
       <c r="C57" s="8">
         <v>44</v>
       </c>
-      <c r="D57" s="29" t="s">
+      <c r="D57" s="28" t="s">
         <v>264</v>
       </c>
       <c r="E57" s="11" t="s">
@@ -5185,7 +5249,7 @@
       <c r="R57" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="S57" s="31" t="s">
+      <c r="S57" s="30" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5226,6 +5290,9 @@
       </c>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
+      <c r="S58" s="39" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="59" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
@@ -5264,6 +5331,9 @@
       </c>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
+      <c r="S59" s="39" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="60" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
@@ -5370,6 +5440,9 @@
       <c r="R62" s="15" t="s">
         <v>184</v>
       </c>
+      <c r="S62" s="39" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
@@ -5403,6 +5476,9 @@
       <c r="Q63" s="10"/>
       <c r="R63" s="15" t="s">
         <v>184</v>
+      </c>
+      <c r="S63" s="39" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="64" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
@@ -5721,10 +5797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF8F5D6-A69C-4604-B31F-611ECF924634}">
-  <dimension ref="B4:P19"/>
+  <dimension ref="B4:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5733,127 +5809,163 @@
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="15:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="O4" s="33" t="s">
+    <row r="4" spans="15:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="O4" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="37" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="5" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O5" s="35" t="s">
+      <c r="Q4" s="30" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O5" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="38" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="6" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O6" s="35" t="s">
+      <c r="Q5" s="38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O6" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="38" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="7" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O7" s="35" t="s">
+      <c r="Q6" s="38" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O7" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="38" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="8" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O8" s="35" t="s">
+      <c r="Q7" s="38" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O8" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="38" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="9" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O9" s="35" t="s">
+      <c r="Q8" s="38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O9" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="38" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="10" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O10" s="35" t="s">
+      <c r="Q9" s="38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O10" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="P10" s="38" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="11" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O11" s="35" t="s">
+      <c r="Q10" s="38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O11" s="33" t="s">
         <v>274</v>
       </c>
-      <c r="P11" s="35" t="s">
+      <c r="P11" s="38" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="12" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O12" s="35" t="s">
+      <c r="Q11" s="38" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O12" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="P12" s="35" t="s">
+      <c r="P12" s="38" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="13" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O13" s="35" t="s">
+      <c r="Q12" s="38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O13" s="33" t="s">
         <v>266</v>
       </c>
-      <c r="P13" s="35" t="s">
+      <c r="P13" s="33" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="14" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O14" s="35" t="s">
+      <c r="Q13" s="40" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O14" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="P14" s="35" t="s">
+      <c r="P14" s="33" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="15" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O15" s="35" t="s">
+      <c r="Q14" s="40" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O15" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="33" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="16" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O16" s="35" t="s">
+      <c r="Q15" s="40" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O16" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="P16" s="36"/>
+      <c r="P16" s="34"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="33" t="s">
         <v>275</v>
       </c>
-      <c r="P17" s="36"/>
+      <c r="P17" s="34"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="35" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="O19" s="32" t="s">
+      <c r="O19" s="31" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5863,6 +5975,7 @@
   </sortState>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated IO xls to reflect all pins.
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELCOT\Platform_2\Platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Platform\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B31D3FC-EE30-4532-93CE-027C1659CBDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A196662-DC6A-4EE0-890C-FC2AAB4D8AED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMD20" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="321">
   <si>
     <r>
       <rPr>
@@ -2674,9 +2674,6 @@
     <t>SWDIO</t>
   </si>
   <si>
-    <t>SPI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enable bit in the Pin Configuration register corresponding to that pin (PINCFGn.PMUXEN, n = 0-31) in the PORT </t>
   </si>
   <si>
@@ -2701,12 +2698,6 @@
     <t>PA18</t>
   </si>
   <si>
-    <t>I2C/SPI</t>
-  </si>
-  <si>
-    <t>I2C</t>
-  </si>
-  <si>
     <t>Already Used for some other puposes</t>
   </si>
   <si>
@@ -2800,9 +2791,6 @@
     <t>C1-Digit Selection</t>
   </si>
   <si>
-    <t>I2C/ADC</t>
-  </si>
-  <si>
     <t>SW4</t>
   </si>
   <si>
@@ -2813,6 +2801,57 @@
   </si>
   <si>
     <t>Use it for Power Input Presence Detection</t>
+  </si>
+  <si>
+    <t>LED_CTRL</t>
+  </si>
+  <si>
+    <t>ESP_UART_TX</t>
+  </si>
+  <si>
+    <t>ESP_UART_RX</t>
+  </si>
+  <si>
+    <t>ESP_EN</t>
+  </si>
+  <si>
+    <t>RTC_SCL</t>
+  </si>
+  <si>
+    <t>RTC_SDA</t>
+  </si>
+  <si>
+    <t>RTC_INT</t>
+  </si>
+  <si>
+    <t>PWR_INP</t>
+  </si>
+  <si>
+    <t>SPI/I2C Header</t>
+  </si>
+  <si>
+    <t>I2C_SDA/ADC</t>
+  </si>
+  <si>
+    <t>I2C_SCL/ADC</t>
+  </si>
+  <si>
+    <t>I2C_SDA</t>
+  </si>
+  <si>
+    <t>I2C_SCL</t>
+  </si>
+  <si>
+    <t>I2C_SCL/SPI_SCK</t>
+  </si>
+  <si>
+    <t>SPI_SS</t>
+  </si>
+  <si>
+    <t>I2C_SDA/SPI_DO</t>
+  </si>
+  <si>
+    <t>SPI_DI</t>
   </si>
 </sst>
 </file>
@@ -3033,7 +3072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3130,9 +3169,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3143,6 +3179,13 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3506,126 +3549,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q58" sqref="Q58"/>
+    <sheetView tabSelected="1" topLeftCell="O9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="4.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="7.109375" customWidth="1"/>
     <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="6.6640625" customWidth="1"/>
+    <col min="18" max="18" width="7.5546875" customWidth="1"/>
+    <col min="19" max="19" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="V2" s="44" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V3" s="44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V4" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V5" s="44" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V6" s="44" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V7" s="44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V8" s="44" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V9" s="44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V11" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V12" s="44" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="V13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V14" s="44" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="V15" s="44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="V17" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="42" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
       <c r="M18" s="7" t="s">
         <v>18</v>
       </c>
@@ -3647,8 +3746,11 @@
       <c r="S18" s="19" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="44" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
@@ -3658,9 +3760,9 @@
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
@@ -3685,18 +3787,21 @@
       <c r="N19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="36" t="s">
+      <c r="O19" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="36"/>
+      <c r="P19" s="42"/>
       <c r="Q19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>1</v>
       </c>
@@ -3734,8 +3839,11 @@
       <c r="S20" s="22" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>2</v>
       </c>
@@ -3773,8 +3881,11 @@
       <c r="S21" s="22" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="44" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>3</v>
       </c>
@@ -3811,11 +3922,14 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
-      <c r="S22" s="41" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="33.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S22" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="V22" s="44" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="33.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>4</v>
       </c>
@@ -3855,8 +3969,11 @@
       <c r="S23" s="22" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V23" s="44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="10"/>
       <c r="C24" s="13">
@@ -3888,8 +4005,9 @@
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="22"/>
-    </row>
-    <row r="25" spans="1:19" ht="12.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V24" s="44"/>
+    </row>
+    <row r="25" spans="1:22" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="10"/>
       <c r="C25" s="13">
@@ -3921,8 +4039,9 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="22"/>
-    </row>
-    <row r="26" spans="1:19" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V25" s="44"/>
+    </row>
+    <row r="26" spans="1:22" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="10"/>
       <c r="C26" s="13">
@@ -3954,8 +4073,9 @@
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="22"/>
-    </row>
-    <row r="27" spans="1:19" ht="12.4" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V26" s="44"/>
+    </row>
+    <row r="27" spans="1:22" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="10"/>
       <c r="C27" s="13">
@@ -3987,8 +4107,9 @@
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="22"/>
-    </row>
-    <row r="28" spans="1:19" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V27" s="44"/>
+    </row>
+    <row r="28" spans="1:22" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="8">
         <v>7</v>
@@ -4025,8 +4146,9 @@
       </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="1:19" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V28" s="44"/>
+    </row>
+    <row r="29" spans="1:22" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="8">
         <v>8</v>
@@ -4063,8 +4185,9 @@
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
-    </row>
-    <row r="30" spans="1:19" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V29" s="44"/>
+    </row>
+    <row r="30" spans="1:22" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>5</v>
       </c>
@@ -4107,11 +4230,14 @@
       </c>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
-      <c r="S30" s="39" t="s">
+      <c r="S30" s="38" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V30" s="44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>6</v>
       </c>
@@ -4152,11 +4278,11 @@
       </c>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
-      <c r="S31" s="39" t="s">
+      <c r="S31" s="38" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>7</v>
       </c>
@@ -4197,11 +4323,11 @@
       </c>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
-      <c r="S32" s="39" t="s">
+      <c r="S32" s="38" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>8</v>
       </c>
@@ -4242,11 +4368,11 @@
       </c>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
-      <c r="S33" s="39" t="s">
+      <c r="S33" s="38" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>11</v>
       </c>
@@ -4257,7 +4383,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>127</v>
@@ -4290,10 +4416,13 @@
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
       <c r="S34" s="30" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="T34" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>12</v>
       </c>
@@ -4304,7 +4433,7 @@
         <v>18</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>135</v>
@@ -4337,10 +4466,13 @@
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
       <c r="S35" s="30" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="T35" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>13</v>
       </c>
@@ -4383,11 +4515,11 @@
       <c r="R36" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="S36" s="39" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S36" s="38" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>14</v>
       </c>
@@ -4430,11 +4562,11 @@
       <c r="R37" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="S37" s="39" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S37" s="38" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="8">
         <v>19</v>
@@ -4470,7 +4602,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="19.7" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="19.649999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="8">
         <v>20</v>
@@ -4506,7 +4638,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8">
@@ -4544,7 +4676,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20"/>
       <c r="B41" s="10"/>
       <c r="C41" s="8">
@@ -4582,7 +4714,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8">
@@ -4618,7 +4750,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="10"/>
       <c r="C43" s="8">
@@ -4654,7 +4786,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="8">
         <v>21</v>
@@ -4694,7 +4826,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="8">
         <v>22</v>
@@ -4734,7 +4866,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>15</v>
       </c>
@@ -4773,14 +4905,14 @@
       <c r="R46" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="S46" s="39" t="s">
-        <v>305</v>
-      </c>
-      <c r="T46" s="42" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S46" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="T46" s="41" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>16</v>
       </c>
@@ -4819,11 +4951,11 @@
       <c r="R47" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="S47" s="39" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S47" s="38" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>17</v>
       </c>
@@ -4834,7 +4966,7 @@
         <v>35</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>127</v>
@@ -4867,10 +4999,13 @@
         <v>199</v>
       </c>
       <c r="S48" s="30" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="T48" s="43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>18</v>
       </c>
@@ -4881,7 +5016,7 @@
         <v>36</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>127</v>
@@ -4914,10 +5049,11 @@
         <v>202</v>
       </c>
       <c r="S49" s="30" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="T49" s="43"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>19</v>
       </c>
@@ -4928,7 +5064,7 @@
         <v>37</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>127</v>
@@ -4959,10 +5095,11 @@
         <v>190</v>
       </c>
       <c r="S50" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="T50" s="43"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>20</v>
       </c>
@@ -5004,10 +5141,11 @@
         <v>192</v>
       </c>
       <c r="S51" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="T51" s="43"/>
+    </row>
+    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21"/>
       <c r="B52" s="10"/>
       <c r="C52" s="8">
@@ -5043,7 +5181,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8">
@@ -5079,7 +5217,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21"/>
       <c r="B54" s="8">
         <v>29</v>
@@ -5119,7 +5257,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
       <c r="B55" s="8">
         <v>30</v>
@@ -5159,7 +5297,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>21</v>
       </c>
@@ -5170,7 +5308,7 @@
         <v>43</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>127</v>
@@ -5203,10 +5341,13 @@
         <v>176</v>
       </c>
       <c r="S56" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="T56" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>22</v>
       </c>
@@ -5217,7 +5358,7 @@
         <v>44</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>127</v>
@@ -5250,10 +5391,13 @@
         <v>180</v>
       </c>
       <c r="S57" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="T57" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>23</v>
       </c>
@@ -5290,11 +5434,11 @@
       </c>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
-      <c r="S58" s="39" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S58" s="38" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>24</v>
       </c>
@@ -5331,11 +5475,11 @@
       </c>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
-      <c r="S59" s="39" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="S59" s="38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21"/>
       <c r="B60" s="8">
         <v>37</v>
@@ -5371,7 +5515,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="21"/>
       <c r="B61" s="8">
         <v>38</v>
@@ -5407,7 +5551,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>25</v>
       </c>
@@ -5440,11 +5584,11 @@
       <c r="R62" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="S62" s="39" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S62" s="38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>27</v>
       </c>
@@ -5477,11 +5621,11 @@
       <c r="R63" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="S63" s="39" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="S63" s="38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>31</v>
       </c>
@@ -5523,8 +5667,11 @@
       <c r="S64" s="23" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="T64" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="13">
         <v>32</v>
       </c>
@@ -5564,8 +5711,11 @@
       <c r="S65" s="24" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T65" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="8">
@@ -5599,7 +5749,7 @@
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
     </row>
-    <row r="67" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="8">
@@ -5633,7 +5783,7 @@
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
     </row>
-    <row r="68" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8">
@@ -5669,7 +5819,7 @@
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
     </row>
-    <row r="69" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="8">
@@ -5705,7 +5855,7 @@
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
     </row>
-    <row r="70" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="18">
         <v>47</v>
@@ -5743,7 +5893,7 @@
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
     </row>
-    <row r="71" spans="1:19" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="18">
         <v>48</v>
@@ -5782,7 +5932,8 @@
       <c r="R71" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="T48:T51"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="D18:D19"/>
@@ -5803,174 +5954,174 @@
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="15:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="15:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="O4" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="P4" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O5" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O6" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O7" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q7" s="37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O8" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q8" s="37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O9" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O10" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="P10" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q10" s="37" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O11" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q11" s="37" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O12" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q12" s="37" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O13" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="P13" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q13" s="39" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O14" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q14" s="39" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O15" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="P15" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q15" s="39" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O16" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="P16" s="34"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="O17" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="P4" s="37" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q4" s="30" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O5" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="P5" s="38" t="s">
-        <v>288</v>
-      </c>
-      <c r="Q5" s="38" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O6" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="P6" s="38" t="s">
+      <c r="P17" s="34"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="Q6" s="38" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O7" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="P7" s="38" t="s">
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="Q7" s="38" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O8" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="P8" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q8" s="38" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O9" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="P9" s="38" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q9" s="38" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O10" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="P10" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q10" s="38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O11" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="P11" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q11" s="38" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O12" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="P12" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q12" s="38" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O13" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="P13" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q13" s="40" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="14" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O14" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="P14" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q14" s="40" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O15" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="P15" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q15" s="40" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="16" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O16" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="P16" s="34"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
-        <v>291</v>
-      </c>
-      <c r="O17" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="P17" s="34"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="35" t="s">
-        <v>293</v>
-      </c>
       <c r="O19" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P5:P15">
+  <sortState ref="P5:P15">
     <sortCondition ref="P5:P15"/>
   </sortState>
   <phoneticPr fontId="23" type="noConversion"/>

</xml_diff>

<commit_message>
updated the schematic as per the latest IO xls.
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Platform\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A196662-DC6A-4EE0-890C-FC2AAB4D8AED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33B27CF-481B-4606-B3FA-7A5EB639B22A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="322">
   <si>
     <r>
       <rPr>
@@ -2794,9 +2794,6 @@
     <t>SW4</t>
   </si>
   <si>
-    <t>SPI-CE</t>
-  </si>
-  <si>
     <t>D2/DAC</t>
   </si>
   <si>
@@ -2852,6 +2849,12 @@
   </si>
   <si>
     <t>SPI_DI</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+  <si>
+    <t>Required</t>
   </si>
 </sst>
 </file>
@@ -3179,13 +3182,13 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3551,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,17 +3591,17 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="44" t="s">
+      <c r="V2" s="42" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="V3" s="44" t="s">
+      <c r="V3" s="42" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="V4" s="44" t="s">
+      <c r="V4" s="42" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3606,7 +3609,7 @@
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="44" t="s">
+      <c r="V5" s="42" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3614,7 +3617,7 @@
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="44" t="s">
+      <c r="V6" s="42" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3622,17 +3625,17 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="44" t="s">
+      <c r="V7" s="42" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="V8" s="44" t="s">
+      <c r="V8" s="42" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="V9" s="44" t="s">
+      <c r="V9" s="42" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3641,23 +3644,23 @@
         <v>5</v>
       </c>
       <c r="V10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="V11" s="44" t="s">
-        <v>305</v>
+      <c r="V11" s="42" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="V12" s="44" t="s">
-        <v>306</v>
+      <c r="V12" s="42" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
@@ -3665,23 +3668,23 @@
         <v>261</v>
       </c>
       <c r="V13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V14" s="44" t="s">
-        <v>308</v>
+      <c r="V14" s="42" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="V15" s="44" t="s">
-        <v>309</v>
+      <c r="V15" s="42" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
@@ -3689,7 +3692,7 @@
         <v>10</v>
       </c>
       <c r="V16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
@@ -3697,34 +3700,34 @@
         <v>11</v>
       </c>
       <c r="V17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="44" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="42" t="s">
+      <c r="H18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
       <c r="M18" s="7" t="s">
         <v>18</v>
       </c>
@@ -3746,7 +3749,7 @@
       <c r="S18" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="V18" s="44" t="s">
+      <c r="V18" s="42" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3760,9 +3763,9 @@
       <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
       <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
@@ -3787,17 +3790,17 @@
       <c r="N19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="42" t="s">
+      <c r="O19" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="P19" s="42"/>
+      <c r="P19" s="44"/>
       <c r="Q19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="V19" s="44" t="s">
+      <c r="V19" s="42" t="s">
         <v>294</v>
       </c>
     </row>
@@ -3839,7 +3842,7 @@
       <c r="S20" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="V20" s="44" t="s">
+      <c r="V20" s="42" t="s">
         <v>295</v>
       </c>
     </row>
@@ -3881,7 +3884,7 @@
       <c r="S21" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="V21" s="44" t="s">
+      <c r="V21" s="42" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3923,9 +3926,9 @@
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="V22" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="V22" s="42" t="s">
         <v>296</v>
       </c>
     </row>
@@ -3969,7 +3972,7 @@
       <c r="S23" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="V23" s="44" t="s">
+      <c r="V23" s="42" t="s">
         <v>297</v>
       </c>
     </row>
@@ -4005,7 +4008,7 @@
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="22"/>
-      <c r="V24" s="44"/>
+      <c r="V24" s="42"/>
     </row>
     <row r="25" spans="1:22" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
@@ -4039,7 +4042,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="22"/>
-      <c r="V25" s="44"/>
+      <c r="V25" s="42"/>
     </row>
     <row r="26" spans="1:22" ht="12.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
@@ -4073,7 +4076,7 @@
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="22"/>
-      <c r="V26" s="44"/>
+      <c r="V26" s="42"/>
     </row>
     <row r="27" spans="1:22" ht="12.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
@@ -4107,7 +4110,7 @@
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="22"/>
-      <c r="V27" s="44"/>
+      <c r="V27" s="42"/>
     </row>
     <row r="28" spans="1:22" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
@@ -4146,7 +4149,7 @@
       </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
-      <c r="V28" s="44"/>
+      <c r="V28" s="42"/>
     </row>
     <row r="29" spans="1:22" ht="19.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
@@ -4185,7 +4188,7 @@
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
-      <c r="V29" s="44"/>
+      <c r="V29" s="42"/>
     </row>
     <row r="30" spans="1:22" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
@@ -4233,7 +4236,7 @@
       <c r="S30" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="V30" s="44" t="s">
+      <c r="V30" s="42" t="s">
         <v>298</v>
       </c>
     </row>
@@ -4327,7 +4330,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>8</v>
       </c>
@@ -4372,7 +4375,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>11</v>
       </c>
@@ -4416,13 +4419,16 @@
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
       <c r="S34" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T34" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+      <c r="U34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>12</v>
       </c>
@@ -4466,13 +4472,16 @@
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
       <c r="S35" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T35" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="U35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>13</v>
       </c>
@@ -4519,7 +4528,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>14</v>
       </c>
@@ -4566,7 +4575,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
       <c r="B38" s="8">
         <v>19</v>
@@ -4602,7 +4611,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="19.649999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="19.649999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="8">
         <v>20</v>
@@ -4638,7 +4647,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="10"/>
       <c r="C40" s="8">
@@ -4676,7 +4685,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20"/>
       <c r="B41" s="10"/>
       <c r="C41" s="8">
@@ -4714,7 +4723,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20"/>
       <c r="B42" s="10"/>
       <c r="C42" s="8">
@@ -4750,7 +4759,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="10"/>
       <c r="C43" s="8">
@@ -4786,7 +4795,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="8">
         <v>21</v>
@@ -4826,7 +4835,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="8">
         <v>22</v>
@@ -4866,7 +4875,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>15</v>
       </c>
@@ -4906,13 +4915,10 @@
         <v>184</v>
       </c>
       <c r="S46" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="T46" s="41" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>16</v>
       </c>
@@ -4952,10 +4958,10 @@
         <v>188</v>
       </c>
       <c r="S47" s="38" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>17</v>
       </c>
@@ -4999,13 +5005,13 @@
         <v>199</v>
       </c>
       <c r="S48" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T48" s="43" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>18</v>
       </c>
@@ -5049,11 +5055,11 @@
         <v>202</v>
       </c>
       <c r="S49" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="T49" s="43"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>19</v>
       </c>
@@ -5095,11 +5101,11 @@
         <v>190</v>
       </c>
       <c r="S50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T50" s="43"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>20</v>
       </c>
@@ -5141,11 +5147,11 @@
         <v>192</v>
       </c>
       <c r="S51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T51" s="43"/>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21"/>
       <c r="B52" s="10"/>
       <c r="C52" s="8">
@@ -5181,7 +5187,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21"/>
       <c r="B53" s="10"/>
       <c r="C53" s="8">
@@ -5217,7 +5223,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21"/>
       <c r="B54" s="8">
         <v>29</v>
@@ -5257,7 +5263,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
       <c r="B55" s="8">
         <v>30</v>
@@ -5297,7 +5303,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>21</v>
       </c>
@@ -5341,13 +5347,16 @@
         <v>176</v>
       </c>
       <c r="S56" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T56" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+      <c r="U56" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>22</v>
       </c>
@@ -5391,13 +5400,16 @@
         <v>180</v>
       </c>
       <c r="S57" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T57" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+      <c r="U57" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>23</v>
       </c>
@@ -5435,10 +5447,13 @@
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="38" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+      <c r="T58" s="41" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>24</v>
       </c>
@@ -5479,7 +5494,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21"/>
       <c r="B60" s="8">
         <v>37</v>
@@ -5515,7 +5530,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="21"/>
       <c r="B61" s="8">
         <v>38</v>
@@ -5551,7 +5566,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>25</v>
       </c>
@@ -5588,7 +5603,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>27</v>
       </c>
@@ -5625,7 +5640,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>31</v>
       </c>
@@ -5668,7 +5683,7 @@
         <v>259</v>
       </c>
       <c r="T64" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.3">
@@ -5712,7 +5727,7 @@
         <v>260</v>
       </c>
       <c r="T65" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added connector for relay controls.
</commit_message>
<xml_diff>
--- a/Platform/SAM D20 Family Data Sheet_IO.xlsx
+++ b/Platform/SAM D20 Family Data Sheet_IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Platform\Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33B27CF-481B-4606-B3FA-7A5EB639B22A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1745B2AC-0A28-47A2-8DF3-21468D55D566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="325">
   <si>
     <r>
       <rPr>
@@ -2855,6 +2855,15 @@
   </si>
   <si>
     <t>Required</t>
+  </si>
+  <si>
+    <t>Relay 1</t>
+  </si>
+  <si>
+    <t>Relay 2</t>
+  </si>
+  <si>
+    <t>Relay 3</t>
   </si>
 </sst>
 </file>
@@ -5010,6 +5019,9 @@
       <c r="T48" s="43" t="s">
         <v>311</v>
       </c>
+      <c r="U48" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
@@ -5058,6 +5070,9 @@
         <v>316</v>
       </c>
       <c r="T49" s="43"/>
+      <c r="U49" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
@@ -5104,6 +5119,9 @@
         <v>317</v>
       </c>
       <c r="T50" s="43"/>
+      <c r="U50" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="13">

</xml_diff>